<commit_message>
Changed filescan.py to account for new folder structure
</commit_message>
<xml_diff>
--- a/tmp_excel_for_merging.xlsx
+++ b/tmp_excel_for_merging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adgceau-my.sharepoint.com/personal/fsaniter_adgce_com/Documents/Desktop/Temp WIP Files/00_QA stuff/adg-qa-check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="8_{F2393E19-B7B4-48F6-B159-0BA71567A11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08EE11D5-CD80-4685-9F3E-0F8895588112}"/>
+  <xr:revisionPtr revIDLastSave="175" documentId="8_{F2393E19-B7B4-48F6-B159-0BA71567A11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A290027D-D292-40D3-A132-F87EE8100906}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="5" xr2:uid="{E5CD7770-9DE5-4B32-A778-9FBAAE9FE817}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="109">
   <si>
     <t>Office</t>
   </si>
@@ -338,6 +338,21 @@
   </si>
   <si>
     <t>\\adgce.local\projects\SSC\27000\27170\CVL\RCRD CPY\2. STAGE 5C\250430_01_STAGE 5C</t>
+  </si>
+  <si>
+    <t>\\adgce.local\projects\SSC\25000\25633\CVL\RCRD CPY\COTTON TREE\250717_01_COTTON TREE IFC</t>
+  </si>
+  <si>
+    <t>\\adgce.local\projects\SSC\27000\27170\CVL\RCRD CPY\2. STAGE 5C\250718_01_IFC W&amp;S</t>
+  </si>
+  <si>
+    <t>\\adgce.local\projects\SSC\27000\27170\CVL\RCRD CPY\4. STAGE 4B\250718_01_IFC W&amp;S</t>
+  </si>
+  <si>
+    <t>\\adgce.local\projects\SSC\27000\27170\CVL\RCRD CPY\3. STAGE 4A\250718_01_IFC W&amp;S</t>
+  </si>
+  <si>
+    <t>\\adgce.local\projects\SSC\27000\27170\CVL\RCRD CPY\1. STAGE 5B\250718_01_IFC W&amp;S</t>
   </si>
 </sst>
 </file>
@@ -2979,10 +2994,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B26D510-B8D3-4FB4-A6AF-DCAE58562D2E}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3492,44 +3507,130 @@
         <v>8</v>
       </c>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:E28">
+  <conditionalFormatting sqref="A2:E33">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E2="Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E28" xr:uid="{C9575B10-2AB5-4CD4-9BD0-242DD2A179F5}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E33" xr:uid="{F5826E85-95F3-4228-A1F6-1F107B395941}">
       <formula1>$J$10:$J$13</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D28" xr:uid="{FA109BA6-27FA-4FCF-9539-D0775A4A7537}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D33" xr:uid="{353C1C33-AA67-4D05-AFFA-654048C49145}">
       <formula1>$J$16:$J$22</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{7F2EC998-B3A7-4AA5-A652-AD8E516530F2}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{7C12A04A-6560-4BBD-A963-737A1387C8ED}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{2C5F3EF3-E1FB-4CDC-9549-97D4A51F2C6A}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{533D1F11-8739-4928-8B2B-A341F728BE23}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{04B38BC5-3CC1-4D3F-B230-1BA92EF9ECAC}"/>
-    <hyperlink ref="C10" r:id="rId6" xr:uid="{F27A410F-B1BE-4A5B-9C11-58AC9C90EA6A}"/>
-    <hyperlink ref="C11" r:id="rId7" xr:uid="{696FAF0C-3027-4B64-822E-4B23516DEE53}"/>
-    <hyperlink ref="C12" r:id="rId8" xr:uid="{5C3DB573-F9DB-4E0D-A732-E73F36E3E482}"/>
-    <hyperlink ref="C20" r:id="rId9" xr:uid="{3667ECB1-7606-44A1-84EF-3ED067F99AC3}"/>
-    <hyperlink ref="C19" r:id="rId10" xr:uid="{2503F897-9992-4849-91B6-B1D3062EA08A}"/>
-    <hyperlink ref="C18" r:id="rId11" xr:uid="{88F0E5C8-FF09-48A3-8B23-B504D03EC6F4}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{5076AA64-EFF8-468C-BE50-EA011BE42E9A}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{D6EF117A-980B-4BDD-9F80-75545CE48C44}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{8CA1FAAB-6014-4B39-BAD7-750EF064FF6D}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{22F32039-FE41-42FF-AB77-E5930E358A64}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{76B65EF1-257B-4825-B84B-0C2F77216EB0}"/>
-    <hyperlink ref="C9" r:id="rId17" xr:uid="{ED41CEAF-134F-4F43-AEE6-F09E70F8FEFC}"/>
-    <hyperlink ref="C6" r:id="rId18" xr:uid="{2FB86A6C-AA42-4EA0-A2CD-C7AE87F2B5AD}"/>
-    <hyperlink ref="C4" r:id="rId19" xr:uid="{9E4746C3-238B-48AB-8C37-6E2F466D6411}"/>
-    <hyperlink ref="C22" r:id="rId20" xr:uid="{2001C54D-633A-40C8-BCAA-C904F5FB69A1}"/>
-    <hyperlink ref="C23" r:id="rId21" xr:uid="{8CA5625B-6DAF-4070-BA5C-3B407E18EB92}"/>
-    <hyperlink ref="C24" r:id="rId22" xr:uid="{24F12447-8997-4D35-B61F-A2600AD99F59}"/>
-    <hyperlink ref="C28" r:id="rId23" xr:uid="{58503F15-4D28-42EC-A34B-18A12D73B941}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{203323E2-C185-403C-98A4-78C908B6CC56}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{ED46B25E-D553-4A37-8E7B-2E42E3027948}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{A87526B3-8785-450C-9FE3-FEFE20838DB7}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{F30BEF85-B5C9-46DB-924E-F0DD7FFA6280}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{8C076C66-5361-4CDD-B39E-05A24BCED446}"/>
+    <hyperlink ref="C10" r:id="rId6" xr:uid="{B5E31079-88AA-4862-88A4-DC3ECBEACE08}"/>
+    <hyperlink ref="C11" r:id="rId7" xr:uid="{B9737EED-BBB6-4427-BE9D-1776A43021BB}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{6665340D-79A4-4A34-85B7-8D50DC51E4DF}"/>
+    <hyperlink ref="C20" r:id="rId9" xr:uid="{86FCCC3C-6EA0-4C23-A9EE-7D8521BE8684}"/>
+    <hyperlink ref="C19" r:id="rId10" xr:uid="{8790BE6B-53E1-4A8F-8E2C-222457FDED68}"/>
+    <hyperlink ref="C18" r:id="rId11" xr:uid="{650098B8-8FFB-48D7-BBB2-84C919329ED2}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{913EFCF1-E071-43D6-BD48-611A5565B62C}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{BA25715F-2F11-4667-92A5-0DE9AD856D7B}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{4329A6E9-78FC-4BDE-B57B-A525BECB02E0}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{D015FEA0-9980-4D30-9DA3-87BDF7560EE7}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{7FA33402-8E15-4EE5-AC93-D7A882697737}"/>
+    <hyperlink ref="C9" r:id="rId17" xr:uid="{5178DEE3-F939-4A03-8518-29419C1C5B2D}"/>
+    <hyperlink ref="C6" r:id="rId18" xr:uid="{9989C864-E171-4FCE-B486-B48A3DF804D5}"/>
+    <hyperlink ref="C4" r:id="rId19" xr:uid="{986943A3-7F61-4861-9857-422553F0ED39}"/>
+    <hyperlink ref="C22" r:id="rId20" xr:uid="{76F7B2FA-D29B-4C79-BAD4-358CF513315F}"/>
+    <hyperlink ref="C23" r:id="rId21" xr:uid="{99C83369-6EC1-4C86-B347-298458BDE716}"/>
+    <hyperlink ref="C24" r:id="rId22" xr:uid="{C3C98FD9-5A57-4D4B-82FF-FF48D18DE102}"/>
+    <hyperlink ref="C28" r:id="rId23" xr:uid="{75521119-C1B1-46B6-AC4A-E6B592DB80FA}"/>
+    <hyperlink ref="C29" r:id="rId24" xr:uid="{E41D56CD-72AC-4306-B132-FECE529749E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3697,9 +3798,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3924,27 +4028,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC3BA9FD-2DD6-4C78-8479-47CB93D20F97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D77A501A-112E-4BCC-A2AE-D214723D105D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="e6f7d2ac-062e-43e3-ae4a-bb8034fa32e1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="fb6a1deb-8c46-45d0-872d-407e6ca3055e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3969,9 +4061,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D77A501A-112E-4BCC-A2AE-D214723D105D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC3BA9FD-2DD6-4C78-8479-47CB93D20F97}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e6f7d2ac-062e-43e3-ae4a-bb8034fa32e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="fb6a1deb-8c46-45d0-872d-407e6ca3055e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>